<commit_message>
Fixing in-spreadsheet tutorial links
</commit_message>
<xml_diff>
--- a/packages/editor/public/assets/documents/script-lab-tutorial.xlsx
+++ b/packages/editor/public/assets/documents/script-lab-tutorial.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18110"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23727"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776AA18C-3506-4514-8426-A9E81E9BCE59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20475" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -23787,47 +23788,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="67" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="24" width="7.7109375" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.265625" customWidth="1"/>
+    <col min="3" max="24" width="7.73046875" customWidth="1"/>
+    <col min="25" max="25" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="3" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="4" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="5" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="6" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="7" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="8" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="9" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="10" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="11" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="12" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="13" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="14" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="15" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="16" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="18" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="19" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="20" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="21" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="22" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="24" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="25" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="26" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="27" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="28" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -23839,43 +23840,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D34" sqref="D34"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="54.7109375" style="4" customWidth="1"/>
-    <col min="2" max="6" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="54.73046875" style="4" customWidth="1"/>
+    <col min="2" max="6" width="9.73046875" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="12:12" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="12:12" ht="60" customHeight="1" x14ac:dyDescent="0.7">
       <c r="L1" s="2"/>
     </row>
-    <row r="5" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="6" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="7" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="8" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="9" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="10" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="17" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5"/>
     </row>
-    <row r="19" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="1:1" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A23" s="6"/>
     </row>
   </sheetData>
@@ -23889,43 +23890,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C16" sqref="C16"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" style="4" customWidth="1"/>
-    <col min="2" max="6" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="50.73046875" style="4" customWidth="1"/>
+    <col min="2" max="6" width="9.1328125" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="12:12" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="12:12" ht="60" customHeight="1" x14ac:dyDescent="0.7">
       <c r="L1" s="2"/>
     </row>
-    <row r="5" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="6" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="7" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="8" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="9" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="10" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="12:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="17" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="7"/>
     </row>
-    <row r="18" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="1:1" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A23" s="6"/>
     </row>
   </sheetData>
@@ -23941,32 +23942,32 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D15" sqref="D15"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="51.3984375" style="4" customWidth="1"/>
     <col min="2" max="6" width="9" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" ht="60" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="6" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="7" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="8" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="9" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="10" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="11" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="15" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="16" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="17" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="18" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="19" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23978,35 +23979,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AK35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G11" sqref="G11"/>
+      <selection pane="topRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" customWidth="1"/>
-    <col min="3" max="24" width="7.7109375" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="50.73046875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.59765625" customWidth="1"/>
+    <col min="3" max="24" width="7.73046875" customWidth="1"/>
+    <col min="25" max="25" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="6" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="7" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="8" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="9" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="10" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="30:37" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AD16" s="4"/>
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
@@ -24016,7 +24017,7 @@
       <c r="AJ16" s="4"/>
       <c r="AK16" s="4"/>
     </row>
-    <row r="17" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" s="1"/>
       <c r="AD17" s="4"/>
       <c r="AE17" s="4"/>
@@ -24027,7 +24028,7 @@
       <c r="AJ17" s="4"/>
       <c r="AK17" s="4"/>
     </row>
-    <row r="18" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AD18" s="4"/>
       <c r="AE18" s="4"/>
       <c r="AF18" s="4"/>
@@ -24037,7 +24038,7 @@
       <c r="AJ18" s="4"/>
       <c r="AK18" s="4"/>
     </row>
-    <row r="19" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
       <c r="AF19" s="4"/>
@@ -24047,7 +24048,7 @@
       <c r="AJ19" s="4"/>
       <c r="AK19" s="4"/>
     </row>
-    <row r="20" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
@@ -24057,7 +24058,7 @@
       <c r="AJ20" s="4"/>
       <c r="AK20" s="4"/>
     </row>
-    <row r="21" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AD21" s="4"/>
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
@@ -24067,7 +24068,7 @@
       <c r="AJ21" s="4"/>
       <c r="AK21" s="4"/>
     </row>
-    <row r="22" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AD22" s="4"/>
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
@@ -24077,7 +24078,7 @@
       <c r="AJ22" s="4"/>
       <c r="AK22" s="4"/>
     </row>
-    <row r="23" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AD23" s="4"/>
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
@@ -24087,7 +24088,7 @@
       <c r="AJ23" s="4"/>
       <c r="AK23" s="4"/>
     </row>
-    <row r="24" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
       <c r="AF24" s="4"/>
@@ -24097,7 +24098,7 @@
       <c r="AJ24" s="4"/>
       <c r="AK24" s="4"/>
     </row>
-    <row r="25" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="L25" s="3"/>
       <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
@@ -24108,7 +24109,7 @@
       <c r="AJ25" s="4"/>
       <c r="AK25" s="4"/>
     </row>
-    <row r="26" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AD26" s="4"/>
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
@@ -24118,7 +24119,7 @@
       <c r="AJ26" s="4"/>
       <c r="AK26" s="4"/>
     </row>
-    <row r="27" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AD27" s="4"/>
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
@@ -24128,7 +24129,7 @@
       <c r="AJ27" s="4"/>
       <c r="AK27" s="4"/>
     </row>
-    <row r="28" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:37" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
       <c r="AF28" s="4"/>
@@ -24138,7 +24139,7 @@
       <c r="AJ28" s="4"/>
       <c r="AK28" s="4"/>
     </row>
-    <row r="29" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:37" x14ac:dyDescent="0.45">
       <c r="AD29" s="4"/>
       <c r="AE29" s="4"/>
       <c r="AF29" s="4"/>
@@ -24148,7 +24149,7 @@
       <c r="AJ29" s="4"/>
       <c r="AK29" s="4"/>
     </row>
-    <row r="30" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:37" x14ac:dyDescent="0.45">
       <c r="AD30" s="4"/>
       <c r="AE30" s="4"/>
       <c r="AF30" s="4"/>
@@ -24158,7 +24159,7 @@
       <c r="AJ30" s="4"/>
       <c r="AK30" s="4"/>
     </row>
-    <row r="31" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:37" x14ac:dyDescent="0.45">
       <c r="AD31" s="4"/>
       <c r="AE31" s="4"/>
       <c r="AF31" s="4"/>
@@ -24168,7 +24169,7 @@
       <c r="AJ31" s="4"/>
       <c r="AK31" s="4"/>
     </row>
-    <row r="32" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:37" x14ac:dyDescent="0.45">
       <c r="AD32" s="4"/>
       <c r="AE32" s="4"/>
       <c r="AF32" s="4"/>
@@ -24178,7 +24179,7 @@
       <c r="AJ32" s="4"/>
       <c r="AK32" s="4"/>
     </row>
-    <row r="33" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="30:37" x14ac:dyDescent="0.45">
       <c r="AD33" s="4"/>
       <c r="AE33" s="4"/>
       <c r="AF33" s="4"/>
@@ -24188,7 +24189,7 @@
       <c r="AJ33" s="4"/>
       <c r="AK33" s="4"/>
     </row>
-    <row r="34" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="30:37" x14ac:dyDescent="0.45">
       <c r="AD34" s="4"/>
       <c r="AE34" s="4"/>
       <c r="AF34" s="4"/>
@@ -24198,7 +24199,7 @@
       <c r="AJ34" s="4"/>
       <c r="AK34" s="4"/>
     </row>
-    <row r="35" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="30:37" x14ac:dyDescent="0.45">
       <c r="AD35" s="4"/>
       <c r="AE35" s="4"/>
       <c r="AF35" s="4"/>

</xml_diff>